<commit_message>
marg bias only for bin cov adjusting for demog
</commit_message>
<xml_diff>
--- a/app/data/hr_sens.xlsx
+++ b/app/data/hr_sens.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2564,6 +2564,4346 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B72">
+        <v>0.946</v>
+      </c>
+      <c r="C72">
+        <v>0.82</v>
+      </c>
+      <c r="D72">
+        <v>1.092</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B73">
+        <v>0.8149999999999999</v>
+      </c>
+      <c r="C73">
+        <v>0.753</v>
+      </c>
+      <c r="D73">
+        <v>0.883</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B74">
+        <v>1.268</v>
+      </c>
+      <c r="C74">
+        <v>1.043</v>
+      </c>
+      <c r="D74">
+        <v>1.542</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>0.988</v>
+      </c>
+      <c r="C75">
+        <v>0.667</v>
+      </c>
+      <c r="D75">
+        <v>1.463</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>2.416</v>
+      </c>
+      <c r="C76">
+        <v>2.307</v>
+      </c>
+      <c r="D76">
+        <v>2.53</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>diabetes</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B77">
+        <v>0.945</v>
+      </c>
+      <c r="C77">
+        <v>0.882</v>
+      </c>
+      <c r="D77">
+        <v>1.013</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>0.847</v>
+      </c>
+      <c r="C78">
+        <v>0.781</v>
+      </c>
+      <c r="D78">
+        <v>0.919</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>0.962</v>
+      </c>
+      <c r="C79">
+        <v>0.888</v>
+      </c>
+      <c r="D79">
+        <v>1.043</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>1.053</v>
+      </c>
+      <c r="C80">
+        <v>0.91</v>
+      </c>
+      <c r="D80">
+        <v>1.217</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B81">
+        <v>0.139</v>
+      </c>
+      <c r="C81">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="D81">
+        <v>0.225</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B82">
+        <v>0.98</v>
+      </c>
+      <c r="C82">
+        <v>0.899</v>
+      </c>
+      <c r="D82">
+        <v>1.068</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B83">
+        <v>1.002</v>
+      </c>
+      <c r="C83">
+        <v>0.897</v>
+      </c>
+      <c r="D83">
+        <v>1.118</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B84">
+        <v>1.482</v>
+      </c>
+      <c r="C84">
+        <v>1.34</v>
+      </c>
+      <c r="D84">
+        <v>1.639</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B85">
+        <v>1.043</v>
+      </c>
+      <c r="C85">
+        <v>0.922</v>
+      </c>
+      <c r="D85">
+        <v>1.181</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B86">
+        <v>1.288</v>
+      </c>
+      <c r="C86">
+        <v>0.971</v>
+      </c>
+      <c r="D86">
+        <v>1.709</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B87">
+        <v>1.968</v>
+      </c>
+      <c r="C87">
+        <v>1.087</v>
+      </c>
+      <c r="D87">
+        <v>3.563</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B88">
+        <v>0.55</v>
+      </c>
+      <c r="C88">
+        <v>0.517</v>
+      </c>
+      <c r="D88">
+        <v>0.585</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>diabetes</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B89">
+        <v>0.983</v>
+      </c>
+      <c r="C89">
+        <v>0.9370000000000001</v>
+      </c>
+      <c r="D89">
+        <v>1.031</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B90">
+        <v>3.048</v>
+      </c>
+      <c r="C90">
+        <v>2.816</v>
+      </c>
+      <c r="D90">
+        <v>3.298</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B91">
+        <v>1.004</v>
+      </c>
+      <c r="C91">
+        <v>0.875</v>
+      </c>
+      <c r="D91">
+        <v>1.153</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B92">
+        <v>1.076</v>
+      </c>
+      <c r="C92">
+        <v>0.969</v>
+      </c>
+      <c r="D92">
+        <v>1.196</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B93">
+        <v>1.106</v>
+      </c>
+      <c r="C93">
+        <v>0.957</v>
+      </c>
+      <c r="D93">
+        <v>1.278</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B94">
+        <v>1.696</v>
+      </c>
+      <c r="C94">
+        <v>1.007</v>
+      </c>
+      <c r="D94">
+        <v>2.858</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B95">
+        <v>0.917</v>
+      </c>
+      <c r="C95">
+        <v>0.79</v>
+      </c>
+      <c r="D95">
+        <v>1.065</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>0.742</v>
+      </c>
+      <c r="C96">
+        <v>0.602</v>
+      </c>
+      <c r="D96">
+        <v>0.915</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B97">
+        <v>0.6</v>
+      </c>
+      <c r="C97">
+        <v>0.537</v>
+      </c>
+      <c r="D97">
+        <v>0.671</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B98">
+        <v>0.775</v>
+      </c>
+      <c r="C98">
+        <v>0.677</v>
+      </c>
+      <c r="D98">
+        <v>0.887</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B99">
+        <v>0.302</v>
+      </c>
+      <c r="C99">
+        <v>0.205</v>
+      </c>
+      <c r="D99">
+        <v>0.444</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>hypoglycemia_hosp</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B100">
+        <v>0.906</v>
+      </c>
+      <c r="C100">
+        <v>0.527</v>
+      </c>
+      <c r="D100">
+        <v>1.557</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>amputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B101">
+        <v>0.745</v>
+      </c>
+      <c r="C101">
+        <v>0.593</v>
+      </c>
+      <c r="D101">
+        <v>0.9370000000000001</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B102">
+        <v>0.502</v>
+      </c>
+      <c r="C102">
+        <v>0.266</v>
+      </c>
+      <c r="D102">
+        <v>0.946</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B103">
+        <v>0.872</v>
+      </c>
+      <c r="C103">
+        <v>0.836</v>
+      </c>
+      <c r="D103">
+        <v>0.909</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B104">
+        <v>0.893</v>
+      </c>
+      <c r="C104">
+        <v>0.797</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B105">
+        <v>0.79</v>
+      </c>
+      <c r="C105">
+        <v>0.708</v>
+      </c>
+      <c r="D105">
+        <v>0.881</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B106">
+        <v>0.927</v>
+      </c>
+      <c r="C106">
+        <v>0.822</v>
+      </c>
+      <c r="D106">
+        <v>1.046</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B107">
+        <v>0.715</v>
+      </c>
+      <c r="C107">
+        <v>0.616</v>
+      </c>
+      <c r="D107">
+        <v>0.831</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B108">
+        <v>1.141</v>
+      </c>
+      <c r="C108">
+        <v>0.478</v>
+      </c>
+      <c r="D108">
+        <v>2.721</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B109">
+        <v>0.946</v>
+      </c>
+      <c r="C109">
+        <v>0.883</v>
+      </c>
+      <c r="D109">
+        <v>1.014</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>retinopathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B110">
+        <v>1.187</v>
+      </c>
+      <c r="C110">
+        <v>0.962</v>
+      </c>
+      <c r="D110">
+        <v>1.464</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B111">
+        <v>1.164</v>
+      </c>
+      <c r="C111">
+        <v>0.946</v>
+      </c>
+      <c r="D111">
+        <v>1.432</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B112">
+        <v>0.362</v>
+      </c>
+      <c r="C112">
+        <v>0.242</v>
+      </c>
+      <c r="D112">
+        <v>0.541</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B113">
+        <v>0.763</v>
+      </c>
+      <c r="C113">
+        <v>0.511</v>
+      </c>
+      <c r="D113">
+        <v>1.139</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B114">
+        <v>0.227</v>
+      </c>
+      <c r="C114">
+        <v>0.059</v>
+      </c>
+      <c r="D114">
+        <v>0.868</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>hypoglycemia_hosp</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B115">
+        <v>1.059</v>
+      </c>
+      <c r="C115">
+        <v>0.429</v>
+      </c>
+      <c r="D115">
+        <v>2.617</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>amputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B116">
+        <v>1.159</v>
+      </c>
+      <c r="C116">
+        <v>0.656</v>
+      </c>
+      <c r="D116">
+        <v>2.047</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B117">
+        <v>0.269</v>
+      </c>
+      <c r="C117">
+        <v>0.035</v>
+      </c>
+      <c r="D117">
+        <v>2.085</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B118">
+        <v>0.906</v>
+      </c>
+      <c r="C118">
+        <v>0.826</v>
+      </c>
+      <c r="D118">
+        <v>0.994</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B119">
+        <v>1.036</v>
+      </c>
+      <c r="C119">
+        <v>0.866</v>
+      </c>
+      <c r="D119">
+        <v>1.239</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B120">
+        <v>0.841</v>
+      </c>
+      <c r="C120">
+        <v>0.645</v>
+      </c>
+      <c r="D120">
+        <v>1.096</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B121">
+        <v>0.789</v>
+      </c>
+      <c r="C121">
+        <v>0.615</v>
+      </c>
+      <c r="D121">
+        <v>1.013</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B122">
+        <v>0.882</v>
+      </c>
+      <c r="C122">
+        <v>0.574</v>
+      </c>
+      <c r="D122">
+        <v>1.353</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B124">
+        <v>0.982</v>
+      </c>
+      <c r="C124">
+        <v>0.851</v>
+      </c>
+      <c r="D124">
+        <v>1.134</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>retinopathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B125">
+        <v>1.072</v>
+      </c>
+      <c r="C125">
+        <v>0.769</v>
+      </c>
+      <c r="D125">
+        <v>1.495</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B126">
+        <v>1.296</v>
+      </c>
+      <c r="C126">
+        <v>0.881</v>
+      </c>
+      <c r="D126">
+        <v>1.908</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B127">
+        <v>0.349</v>
+      </c>
+      <c r="C127">
+        <v>0.299</v>
+      </c>
+      <c r="D127">
+        <v>0.406</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B128">
+        <v>0.662</v>
+      </c>
+      <c r="C128">
+        <v>0.569</v>
+      </c>
+      <c r="D128">
+        <v>0.77</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B129">
+        <v>0.162</v>
+      </c>
+      <c r="C129">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D129">
+        <v>0.296</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>hypoglycemia_hosp</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B130">
+        <v>0.496</v>
+      </c>
+      <c r="C130">
+        <v>0.252</v>
+      </c>
+      <c r="D130">
+        <v>0.978</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>amputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B131">
+        <v>0.798</v>
+      </c>
+      <c r="C131">
+        <v>0.635</v>
+      </c>
+      <c r="D131">
+        <v>1.002</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B132">
+        <v>0.138</v>
+      </c>
+      <c r="C132">
+        <v>0.046</v>
+      </c>
+      <c r="D132">
+        <v>0.41</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B133">
+        <v>0.832</v>
+      </c>
+      <c r="C133">
+        <v>0.796</v>
+      </c>
+      <c r="D133">
+        <v>0.87</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B134">
+        <v>0.931</v>
+      </c>
+      <c r="C134">
+        <v>0.832</v>
+      </c>
+      <c r="D134">
+        <v>1.041</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B135">
+        <v>0.768</v>
+      </c>
+      <c r="C135">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="D135">
+        <v>0.863</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B136">
+        <v>0.851</v>
+      </c>
+      <c r="C136">
+        <v>0.747</v>
+      </c>
+      <c r="D136">
+        <v>0.97</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B137">
+        <v>0.91</v>
+      </c>
+      <c r="C137">
+        <v>0.779</v>
+      </c>
+      <c r="D137">
+        <v>1.063</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B138">
+        <v>0.103</v>
+      </c>
+      <c r="C138">
+        <v>0.013</v>
+      </c>
+      <c r="D138">
+        <v>0.845</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B139">
+        <v>0.953</v>
+      </c>
+      <c r="C139">
+        <v>0.888</v>
+      </c>
+      <c r="D139">
+        <v>1.022</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>retinopathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B140">
+        <v>1.163</v>
+      </c>
+      <c r="C140">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="D140">
+        <v>1.44</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B141">
+        <v>1.041</v>
+      </c>
+      <c r="C141">
+        <v>0.838</v>
+      </c>
+      <c r="D141">
+        <v>1.294</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B142">
+        <v>0.946</v>
+      </c>
+      <c r="C142">
+        <v>0.82</v>
+      </c>
+      <c r="D142">
+        <v>1.092</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B143">
+        <v>0.8149999999999999</v>
+      </c>
+      <c r="C143">
+        <v>0.753</v>
+      </c>
+      <c r="D143">
+        <v>0.883</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B144">
+        <v>1.268</v>
+      </c>
+      <c r="C144">
+        <v>1.043</v>
+      </c>
+      <c r="D144">
+        <v>1.542</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B145">
+        <v>0.988</v>
+      </c>
+      <c r="C145">
+        <v>0.667</v>
+      </c>
+      <c r="D145">
+        <v>1.463</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B146">
+        <v>2.416</v>
+      </c>
+      <c r="C146">
+        <v>2.307</v>
+      </c>
+      <c r="D146">
+        <v>2.53</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>diabetes</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B147">
+        <v>0.945</v>
+      </c>
+      <c r="C147">
+        <v>0.882</v>
+      </c>
+      <c r="D147">
+        <v>1.013</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B148">
+        <v>0.847</v>
+      </c>
+      <c r="C148">
+        <v>0.781</v>
+      </c>
+      <c r="D148">
+        <v>0.919</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B149">
+        <v>0.962</v>
+      </c>
+      <c r="C149">
+        <v>0.888</v>
+      </c>
+      <c r="D149">
+        <v>1.043</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B150">
+        <v>1.053</v>
+      </c>
+      <c r="C150">
+        <v>0.91</v>
+      </c>
+      <c r="D150">
+        <v>1.217</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B151">
+        <v>0.139</v>
+      </c>
+      <c r="C151">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="D151">
+        <v>0.225</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B152">
+        <v>0.98</v>
+      </c>
+      <c r="C152">
+        <v>0.899</v>
+      </c>
+      <c r="D152">
+        <v>1.068</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B153">
+        <v>1.002</v>
+      </c>
+      <c r="C153">
+        <v>0.897</v>
+      </c>
+      <c r="D153">
+        <v>1.118</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>arb_vs_acei</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B154">
+        <v>1.482</v>
+      </c>
+      <c r="C154">
+        <v>1.34</v>
+      </c>
+      <c r="D154">
+        <v>1.639</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B155">
+        <v>1.043</v>
+      </c>
+      <c r="C155">
+        <v>0.922</v>
+      </c>
+      <c r="D155">
+        <v>1.181</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B156">
+        <v>1.288</v>
+      </c>
+      <c r="C156">
+        <v>0.971</v>
+      </c>
+      <c r="D156">
+        <v>1.709</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B157">
+        <v>1.968</v>
+      </c>
+      <c r="C157">
+        <v>1.087</v>
+      </c>
+      <c r="D157">
+        <v>3.563</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B158">
+        <v>0.55</v>
+      </c>
+      <c r="C158">
+        <v>0.517</v>
+      </c>
+      <c r="D158">
+        <v>0.585</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>diabetes</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B159">
+        <v>0.983</v>
+      </c>
+      <c r="C159">
+        <v>0.9370000000000001</v>
+      </c>
+      <c r="D159">
+        <v>1.031</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B160">
+        <v>3.048</v>
+      </c>
+      <c r="C160">
+        <v>2.816</v>
+      </c>
+      <c r="D160">
+        <v>3.298</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B161">
+        <v>1.004</v>
+      </c>
+      <c r="C161">
+        <v>0.875</v>
+      </c>
+      <c r="D161">
+        <v>1.153</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B162">
+        <v>1.076</v>
+      </c>
+      <c r="C162">
+        <v>0.969</v>
+      </c>
+      <c r="D162">
+        <v>1.196</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B163">
+        <v>1.106</v>
+      </c>
+      <c r="C163">
+        <v>0.957</v>
+      </c>
+      <c r="D163">
+        <v>1.278</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B164">
+        <v>1.696</v>
+      </c>
+      <c r="C164">
+        <v>1.007</v>
+      </c>
+      <c r="D164">
+        <v>2.858</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B165">
+        <v>0.917</v>
+      </c>
+      <c r="C165">
+        <v>0.79</v>
+      </c>
+      <c r="D165">
+        <v>1.065</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B166">
+        <v>0.742</v>
+      </c>
+      <c r="C166">
+        <v>0.602</v>
+      </c>
+      <c r="D166">
+        <v>0.915</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>snri_vs_ssri</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B167">
+        <v>0.6</v>
+      </c>
+      <c r="C167">
+        <v>0.537</v>
+      </c>
+      <c r="D167">
+        <v>0.671</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B168">
+        <v>0.775</v>
+      </c>
+      <c r="C168">
+        <v>0.677</v>
+      </c>
+      <c r="D168">
+        <v>0.887</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B169">
+        <v>0.302</v>
+      </c>
+      <c r="C169">
+        <v>0.205</v>
+      </c>
+      <c r="D169">
+        <v>0.444</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>hypoglycemia_hosp</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B170">
+        <v>0.906</v>
+      </c>
+      <c r="C170">
+        <v>0.527</v>
+      </c>
+      <c r="D170">
+        <v>1.557</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>amputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B171">
+        <v>0.745</v>
+      </c>
+      <c r="C171">
+        <v>0.593</v>
+      </c>
+      <c r="D171">
+        <v>0.9370000000000001</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B172">
+        <v>0.502</v>
+      </c>
+      <c r="C172">
+        <v>0.266</v>
+      </c>
+      <c r="D172">
+        <v>0.946</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B173">
+        <v>0.872</v>
+      </c>
+      <c r="C173">
+        <v>0.836</v>
+      </c>
+      <c r="D173">
+        <v>0.909</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B174">
+        <v>0.893</v>
+      </c>
+      <c r="C174">
+        <v>0.797</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B175">
+        <v>0.79</v>
+      </c>
+      <c r="C175">
+        <v>0.708</v>
+      </c>
+      <c r="D175">
+        <v>0.881</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B176">
+        <v>0.927</v>
+      </c>
+      <c r="C176">
+        <v>0.822</v>
+      </c>
+      <c r="D176">
+        <v>1.046</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B177">
+        <v>0.715</v>
+      </c>
+      <c r="C177">
+        <v>0.616</v>
+      </c>
+      <c r="D177">
+        <v>0.831</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B178">
+        <v>1.141</v>
+      </c>
+      <c r="C178">
+        <v>0.478</v>
+      </c>
+      <c r="D178">
+        <v>2.721</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B179">
+        <v>0.946</v>
+      </c>
+      <c r="C179">
+        <v>0.883</v>
+      </c>
+      <c r="D179">
+        <v>1.014</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>retinopathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B180">
+        <v>1.187</v>
+      </c>
+      <c r="C180">
+        <v>0.962</v>
+      </c>
+      <c r="D180">
+        <v>1.464</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B181">
+        <v>1.164</v>
+      </c>
+      <c r="C181">
+        <v>0.946</v>
+      </c>
+      <c r="D181">
+        <v>1.432</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>su_vs_dpp4</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B182">
+        <v>0.362</v>
+      </c>
+      <c r="C182">
+        <v>0.242</v>
+      </c>
+      <c r="D182">
+        <v>0.541</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B183">
+        <v>0.763</v>
+      </c>
+      <c r="C183">
+        <v>0.511</v>
+      </c>
+      <c r="D183">
+        <v>1.139</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B184">
+        <v>0.227</v>
+      </c>
+      <c r="C184">
+        <v>0.059</v>
+      </c>
+      <c r="D184">
+        <v>0.868</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>hypoglycemia_hosp</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B185">
+        <v>1.059</v>
+      </c>
+      <c r="C185">
+        <v>0.429</v>
+      </c>
+      <c r="D185">
+        <v>2.617</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>amputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B186">
+        <v>1.159</v>
+      </c>
+      <c r="C186">
+        <v>0.656</v>
+      </c>
+      <c r="D186">
+        <v>2.047</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B187">
+        <v>0.269</v>
+      </c>
+      <c r="C187">
+        <v>0.035</v>
+      </c>
+      <c r="D187">
+        <v>2.085</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B188">
+        <v>0.906</v>
+      </c>
+      <c r="C188">
+        <v>0.826</v>
+      </c>
+      <c r="D188">
+        <v>0.994</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B189">
+        <v>1.036</v>
+      </c>
+      <c r="C189">
+        <v>0.866</v>
+      </c>
+      <c r="D189">
+        <v>1.239</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B190">
+        <v>0.841</v>
+      </c>
+      <c r="C190">
+        <v>0.645</v>
+      </c>
+      <c r="D190">
+        <v>1.096</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B191">
+        <v>0.789</v>
+      </c>
+      <c r="C191">
+        <v>0.615</v>
+      </c>
+      <c r="D191">
+        <v>1.013</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B192">
+        <v>0.882</v>
+      </c>
+      <c r="C192">
+        <v>0.574</v>
+      </c>
+      <c r="D192">
+        <v>1.353</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B194">
+        <v>0.982</v>
+      </c>
+      <c r="C194">
+        <v>0.851</v>
+      </c>
+      <c r="D194">
+        <v>1.134</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>retinopathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B195">
+        <v>1.072</v>
+      </c>
+      <c r="C195">
+        <v>0.769</v>
+      </c>
+      <c r="D195">
+        <v>1.495</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B196">
+        <v>1.296</v>
+      </c>
+      <c r="C196">
+        <v>0.881</v>
+      </c>
+      <c r="D196">
+        <v>1.908</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>su_vs_glp1</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B197">
+        <v>0.349</v>
+      </c>
+      <c r="C197">
+        <v>0.299</v>
+      </c>
+      <c r="D197">
+        <v>0.406</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B198">
+        <v>0.662</v>
+      </c>
+      <c r="C198">
+        <v>0.569</v>
+      </c>
+      <c r="D198">
+        <v>0.77</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>stroke</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B199">
+        <v>0.162</v>
+      </c>
+      <c r="C199">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="D199">
+        <v>0.296</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>hypoglycemia_hosp</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B200">
+        <v>0.496</v>
+      </c>
+      <c r="C200">
+        <v>0.252</v>
+      </c>
+      <c r="D200">
+        <v>0.978</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>amputation</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B201">
+        <v>0.798</v>
+      </c>
+      <c r="C201">
+        <v>0.635</v>
+      </c>
+      <c r="D201">
+        <v>1.002</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B202">
+        <v>0.138</v>
+      </c>
+      <c r="C202">
+        <v>0.046</v>
+      </c>
+      <c r="D202">
+        <v>0.41</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>copd_exacerbation</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B203">
+        <v>0.832</v>
+      </c>
+      <c r="C203">
+        <v>0.796</v>
+      </c>
+      <c r="D203">
+        <v>0.87</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>hypertension</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B204">
+        <v>0.931</v>
+      </c>
+      <c r="C204">
+        <v>0.832</v>
+      </c>
+      <c r="D204">
+        <v>1.041</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>depression</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B205">
+        <v>0.768</v>
+      </c>
+      <c r="C205">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="D205">
+        <v>0.863</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>hyperlipidemia</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B206">
+        <v>0.851</v>
+      </c>
+      <c r="C206">
+        <v>0.747</v>
+      </c>
+      <c r="D206">
+        <v>0.97</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>copd</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B207">
+        <v>0.91</v>
+      </c>
+      <c r="C207">
+        <v>0.779</v>
+      </c>
+      <c r="D207">
+        <v>1.063</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>chf</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B208">
+        <v>0.103</v>
+      </c>
+      <c r="C208">
+        <v>0.013</v>
+      </c>
+      <c r="D208">
+        <v>0.845</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>end_stage_renal</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B209">
+        <v>0.953</v>
+      </c>
+      <c r="C209">
+        <v>0.888</v>
+      </c>
+      <c r="D209">
+        <v>1.022</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>retinopathy</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B210">
+        <v>1.163</v>
+      </c>
+      <c r="C210">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="D210">
+        <v>1.44</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>breast_cancer_screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>AT_sens</t>
+        </is>
+      </c>
+      <c r="B211">
+        <v>1.041</v>
+      </c>
+      <c r="C211">
+        <v>0.838</v>
+      </c>
+      <c r="D211">
+        <v>1.294</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>cprd</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>su_vs_sglt2</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>colon_cancer_screen</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>